<commit_message>
New version of RACI
</commit_message>
<xml_diff>
--- a/Montage/RACI.xlsx
+++ b/Montage/RACI.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="30">
   <si>
     <t>Tom</t>
   </si>
@@ -40,9 +40,6 @@
     <t>R</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Affichage page recherche</t>
   </si>
   <si>
@@ -64,19 +61,22 @@
     <t>Systeme de tags</t>
   </si>
   <si>
+    <t>A</t>
+  </si>
+  <si>
     <t>Recherche lexicographique</t>
   </si>
   <si>
     <t>Système de vote (réaction)</t>
   </si>
   <si>
+    <t>C</t>
+  </si>
+  <si>
     <t>Base de donnée des projets</t>
   </si>
   <si>
     <t>Base de donnée utilisateur</t>
-  </si>
-  <si>
-    <t>Base de donnée sondage</t>
   </si>
   <si>
     <t>Algotithme de Login</t>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>Sondage</t>
+  </si>
+  <si>
+    <t>Base de donnée sondage</t>
   </si>
   <si>
     <t>R = réalisation</t>
@@ -491,10 +494,10 @@
         <v>6</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -520,7 +523,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>8</v>
@@ -529,10 +532,10 @@
         <v>6</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -558,7 +561,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>8</v>
@@ -567,10 +570,10 @@
         <v>6</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -596,7 +599,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>8</v>
@@ -605,10 +608,10 @@
         <v>6</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -634,7 +637,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>8</v>
@@ -643,10 +646,10 @@
         <v>6</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -672,19 +675,19 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -710,19 +713,19 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -748,19 +751,19 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -792,13 +795,13 @@
         <v>6</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -827,18 +830,18 @@
         <v>18</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="D12" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
-      <c r="F12" s="3"/>
+      <c r="F12" s="5"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
@@ -862,21 +865,21 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="D13" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
-      <c r="F13" s="3"/>
+      <c r="F13" s="5"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -900,21 +903,21 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="D14" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
-      <c r="F14" s="3"/>
+      <c r="F14" s="5"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -938,19 +941,19 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -976,20 +979,12 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -1014,20 +1009,12 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -1052,20 +1039,12 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -1124,7 +1103,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
@@ -1154,7 +1133,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
@@ -1184,7 +1163,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
@@ -1214,7 +1193,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>

</xml_diff>